<commit_message>
updated cv and syllabi
</commit_message>
<xml_diff>
--- a/assets/CV/pubs.xlsx
+++ b/assets/CV/pubs.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tysonbarrett/Dropbox/GitHub/blog_rstats/assets/CV/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CCD2CBD-8B5A-DB4B-B66E-627927B04F99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BB55DA5-36BD-8C41-89B3-1B6B0AE746D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="36880" yWindow="2220" windowWidth="28800" windowHeight="16520" xr2:uid="{D694CAF4-E52C-7242-8187-CC366AD31369}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="234">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="237">
   <si>
     <t>authors</t>
   </si>
@@ -737,6 +737,15 @@
   </si>
   <si>
     <t>Petersen, J. M., Barney, J. L., Barrett, T. S., Lensegrav-Benson, T., Quakenbush-Roberts, B., &amp; Twohig, M. P. </t>
+  </si>
+  <si>
+    <t>Barney, J. L., Barrett, T. S., Lensegrav-Benson, T., Quakenbush, B., Twohig, M. P.</t>
+  </si>
+  <si>
+    <t>Examining a mediation model of body image-related cognitive fusion, intuitive eating, and eating disorder symptom severity in a clinical sample.</t>
+  </si>
+  <si>
+    <t>Eating and Weight Disorders – Studies on Anorexia, Bulimia, and Obesity</t>
   </si>
 </sst>
 </file>
@@ -1122,10 +1131,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38BAB23D-B27F-A34D-A522-4C115B575C05}">
-  <dimension ref="A1:I52"/>
+  <dimension ref="A1:I53"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1186,1125 +1195,1116 @@
       </c>
     </row>
     <row r="3" spans="1:9" ht="51" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
-        <v>158</v>
+      <c r="A3" s="6" t="s">
+        <v>234</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>143</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>230</v>
+        <v>235</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>157</v>
+        <v>236</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>143</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>152</v>
+        <v>230</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" ht="68" x14ac:dyDescent="0.2">
+        <v>153</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>143</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>150</v>
+        <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="68" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="68" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
         <v>161</v>
-      </c>
-      <c r="B6" s="1">
-        <v>2021</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="E6" s="1">
-        <v>131</v>
-      </c>
-      <c r="G6" s="4" t="s">
-        <v>229</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" ht="51" x14ac:dyDescent="0.2">
-      <c r="A7" s="1" t="s">
-        <v>162</v>
       </c>
       <c r="B7" s="1">
         <v>2021</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>203</v>
+        <v>146</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>144</v>
+        <v>147</v>
+      </c>
+      <c r="E7" s="1">
+        <v>131</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>229</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" ht="68" x14ac:dyDescent="0.2">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B8" s="1">
         <v>2021</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>149</v>
+        <v>203</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="E8" s="5">
-        <v>16</v>
-      </c>
-      <c r="F8" s="1">
-        <v>10</v>
-      </c>
-      <c r="G8" s="4" t="s">
-        <v>155</v>
+        <v>144</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" ht="51" x14ac:dyDescent="0.2">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="68" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B9" s="1">
         <v>2021</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>5</v>
+        <v>149</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E9" s="1">
-        <v>38</v>
+        <v>148</v>
+      </c>
+      <c r="E9" s="5">
+        <v>16</v>
+      </c>
+      <c r="F9" s="1">
+        <v>10</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>119</v>
+        <v>155</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" ht="68" x14ac:dyDescent="0.2">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B10" s="1">
         <v>2021</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>204</v>
+        <v>5</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>113</v>
+        <v>6</v>
+      </c>
+      <c r="E10" s="1">
+        <v>38</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>111</v>
+        <v>119</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" ht="51" x14ac:dyDescent="0.2">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="68" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B11" s="1">
         <v>2021</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>7</v>
+        <v>204</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="F11" s="1">
-        <v>1</v>
+        <v>113</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="I11" s="1" t="s">
-        <v>96</v>
+        <v>114</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B12" s="1">
         <v>2021</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E12" s="1">
-        <v>77</v>
+        <v>8</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>115</v>
       </c>
       <c r="F12" s="1">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>145</v>
+        <v>116</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>112</v>
+        <v>117</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B13" s="1">
         <v>2021</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>205</v>
+        <v>9</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
+      </c>
+      <c r="E13" s="1">
+        <v>77</v>
+      </c>
+      <c r="F13" s="1">
+        <v>10</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>110</v>
-      </c>
-      <c r="I13" s="1" t="s">
-        <v>97</v>
+        <v>145</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B14" s="1">
         <v>2021</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>12</v>
+        <v>205</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>11</v>
       </c>
       <c r="G14" s="4" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" ht="68" x14ac:dyDescent="0.2">
+        <v>110</v>
+      </c>
+      <c r="I14" s="1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B15" s="1">
         <v>2021</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>206</v>
+        <v>12</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="H15" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="I15" s="1" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" ht="51" x14ac:dyDescent="0.2">
+        <v>11</v>
+      </c>
+      <c r="G15" s="4" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="68" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B16" s="1">
         <v>2021</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>11</v>
+        <v>95</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" ht="68" x14ac:dyDescent="0.2">
+        <v>120</v>
+      </c>
+      <c r="I16" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B17" s="1">
         <v>2021</v>
       </c>
       <c r="C17" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="68" x14ac:dyDescent="0.2">
+      <c r="A18" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="B18" s="1">
+        <v>2021</v>
+      </c>
+      <c r="C18" s="1" t="s">
         <v>208</v>
       </c>
-      <c r="D17" s="1" t="s">
+      <c r="D18" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="H17" s="1" t="s">
+      <c r="H18" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="I17" s="1" t="s">
+      <c r="I18" s="1" t="s">
         <v>99</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" ht="51" x14ac:dyDescent="0.2">
-      <c r="A18" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="B18" s="1">
-        <v>2020</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E18" s="1">
-        <v>42</v>
-      </c>
-      <c r="G18" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="H18" s="1" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="19" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B19" s="1">
         <v>2020</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="E19" s="1">
-        <v>18</v>
+        <v>42</v>
       </c>
       <c r="G19" s="4" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="20" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B20" s="1">
         <v>2020</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="E20" s="1">
-        <v>63</v>
-      </c>
-      <c r="F20" s="1">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="G20" s="4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="21" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B21" s="1">
         <v>2020</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>209</v>
+        <v>25</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>27</v>
+        <v>11</v>
       </c>
       <c r="E21" s="1">
-        <v>40</v>
+        <v>63</v>
+      </c>
+      <c r="F21" s="1">
+        <v>6</v>
       </c>
       <c r="G21" s="4" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="I21" s="1" t="s">
-        <v>109</v>
+        <v>124</v>
       </c>
     </row>
     <row r="22" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B22" s="1">
         <v>2020</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E22" s="1">
-        <v>51</v>
-      </c>
-      <c r="F22" s="1">
-        <v>3</v>
+        <v>40</v>
       </c>
       <c r="G22" s="4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="I22" s="1" t="s">
-        <v>100</v>
+        <v>109</v>
       </c>
     </row>
     <row r="23" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B23" s="1">
         <v>2020</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>31</v>
+        <v>210</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>11</v>
+        <v>29</v>
       </c>
       <c r="E23" s="1">
-        <v>63</v>
+        <v>51</v>
       </c>
       <c r="F23" s="1">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="G23" s="4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
+      </c>
+      <c r="I23" s="1" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="24" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B24" s="1">
         <v>2020</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>211</v>
+        <v>31</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="E24" s="1">
-        <v>51</v>
+        <v>63</v>
       </c>
       <c r="F24" s="1">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="G24" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="25" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B25" s="1">
         <v>2020</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="E25" s="1">
-        <v>21</v>
+        <v>51</v>
       </c>
       <c r="F25" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G25" s="4" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" ht="68" x14ac:dyDescent="0.2">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B26" s="1">
         <v>2020</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E26" s="1">
-        <v>113</v>
+        <v>21</v>
       </c>
       <c r="F26" s="1">
         <v>2</v>
       </c>
       <c r="G26" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="H26" s="1" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" ht="68" x14ac:dyDescent="0.2">
+      <c r="A27" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="B27" s="1">
+        <v>2020</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E27" s="1">
+        <v>113</v>
+      </c>
+      <c r="F27" s="1">
+        <v>2</v>
+      </c>
+      <c r="G27" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="H26" s="1" t="s">
+      <c r="H27" s="1" t="s">
         <v>130</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" ht="51" x14ac:dyDescent="0.2">
-      <c r="A27" s="1" t="s">
-        <v>182</v>
-      </c>
-      <c r="B27" s="1">
-        <v>2019</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="D27" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="E27" s="1">
-        <v>61</v>
-      </c>
-      <c r="F27" s="1">
-        <v>3</v>
-      </c>
-      <c r="G27" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="H27" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="I27" s="1" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="28" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B28" s="1">
         <v>2019</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>11</v>
+        <v>39</v>
       </c>
       <c r="E28" s="1">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F28" s="1">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="G28" s="4" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="H28" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
+      </c>
+      <c r="I28" s="1" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="29" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B29" s="1">
         <v>2019</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>44</v>
+        <v>11</v>
       </c>
       <c r="E29" s="1">
-        <v>10</v>
+        <v>62</v>
       </c>
       <c r="F29" s="1">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="G29" s="4" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="H29" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="I29" s="1" t="s">
-        <v>102</v>
+        <v>132</v>
       </c>
     </row>
     <row r="30" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B30" s="1">
         <v>2019</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>23</v>
+        <v>44</v>
       </c>
       <c r="E30" s="1">
-        <v>13</v>
+        <v>10</v>
+      </c>
+      <c r="F30" s="1">
+        <v>10</v>
       </c>
       <c r="G30" s="4" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="H30" s="1" t="s">
-        <v>136</v>
+        <v>133</v>
+      </c>
+      <c r="I30" s="1" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="31" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B31" s="1">
         <v>2019</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>48</v>
+        <v>23</v>
       </c>
       <c r="E31" s="1">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="G31" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="H31" s="1" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
     </row>
     <row r="32" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B32" s="1">
         <v>2019</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>214</v>
+        <v>47</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
       <c r="E32" s="1">
-        <v>20</v>
-      </c>
-      <c r="F32" s="1">
-        <v>4</v>
+        <v>22</v>
       </c>
       <c r="G32" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H32" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="I32" s="1" t="s">
-        <v>103</v>
+        <v>134</v>
       </c>
     </row>
     <row r="33" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B33" s="1">
         <v>2019</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>52</v>
+        <v>214</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>53</v>
+        <v>34</v>
+      </c>
+      <c r="E33" s="1">
+        <v>20</v>
+      </c>
+      <c r="F33" s="1">
+        <v>4</v>
       </c>
       <c r="G33" s="4" t="s">
-        <v>215</v>
+        <v>51</v>
       </c>
       <c r="H33" s="1" t="s">
-        <v>137</v>
+        <v>135</v>
+      </c>
+      <c r="I33" s="1" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="34" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B34" s="1">
         <v>2019</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="E34" s="1">
-        <v>145</v>
-      </c>
-      <c r="F34" s="1">
-        <v>1</v>
+        <v>53</v>
       </c>
       <c r="G34" s="4" t="s">
-        <v>55</v>
+        <v>215</v>
       </c>
       <c r="H34" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="I34" s="1" t="s">
-        <v>104</v>
+        <v>137</v>
       </c>
     </row>
     <row r="35" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B35" s="1">
         <v>2019</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>57</v>
+        <v>39</v>
       </c>
       <c r="E35" s="1">
-        <v>81</v>
+        <v>145</v>
       </c>
       <c r="F35" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G35" s="4" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9" ht="68" x14ac:dyDescent="0.2">
+        <v>55</v>
+      </c>
+      <c r="H35" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="I35" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B36" s="1">
         <v>2019</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>11</v>
+        <v>57</v>
       </c>
       <c r="E36" s="1">
-        <v>62</v>
+        <v>81</v>
       </c>
       <c r="F36" s="1">
         <v>2</v>
       </c>
       <c r="G36" s="4" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" ht="68" x14ac:dyDescent="0.2">
+      <c r="A37" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="B37" s="1">
+        <v>2019</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E37" s="1">
+        <v>62</v>
+      </c>
+      <c r="F37" s="1">
+        <v>2</v>
+      </c>
+      <c r="G37" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="I36" s="1" t="s">
+      <c r="I37" s="1" t="s">
         <v>105</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9" ht="51" x14ac:dyDescent="0.2">
-      <c r="A37" s="1" t="s">
-        <v>192</v>
-      </c>
-      <c r="B37" s="1">
-        <v>2018</v>
-      </c>
-      <c r="C37" s="1" t="s">
-        <v>216</v>
-      </c>
-      <c r="D37" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="E37" s="1">
-        <v>3</v>
-      </c>
-      <c r="F37" s="1">
-        <v>1</v>
-      </c>
-      <c r="G37" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="I37" s="1" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="38" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B38" s="1">
         <v>2018</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>64</v>
+        <v>216</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="E38" s="1">
-        <v>143</v>
+        <v>3</v>
       </c>
       <c r="F38" s="1">
-        <v>3</v>
-      </c>
-      <c r="H38" s="1" t="s">
-        <v>138</v>
+        <v>1</v>
+      </c>
+      <c r="G38" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="I38" s="1" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="39" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
-        <v>168</v>
+        <v>193</v>
       </c>
       <c r="B39" s="1">
         <v>2018</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E39" s="1">
         <v>143</v>
       </c>
       <c r="F39" s="1">
+        <v>3</v>
+      </c>
+      <c r="H39" s="1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" ht="51" x14ac:dyDescent="0.2">
+      <c r="A40" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B40" s="1">
+        <v>2018</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E40" s="1">
+        <v>143</v>
+      </c>
+      <c r="F40" s="1">
         <v>5</v>
       </c>
-      <c r="H39" s="1" t="s">
+      <c r="H40" s="1" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="40" spans="1:9" ht="68" x14ac:dyDescent="0.2">
-      <c r="A40" s="1" t="s">
+    <row r="41" spans="1:9" ht="68" x14ac:dyDescent="0.2">
+      <c r="A41" s="1" t="s">
         <v>194</v>
-      </c>
-      <c r="B40" s="1">
-        <v>2017</v>
-      </c>
-      <c r="C40" s="1" t="s">
-        <v>217</v>
-      </c>
-      <c r="D40" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="E40" s="1">
-        <v>9</v>
-      </c>
-      <c r="F40" s="1">
-        <v>2</v>
-      </c>
-      <c r="G40" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="I40" s="1" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9" ht="51" x14ac:dyDescent="0.2">
-      <c r="A41" s="1" t="s">
-        <v>168</v>
       </c>
       <c r="B41" s="1">
         <v>2017</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>11</v>
+        <v>68</v>
       </c>
       <c r="E41" s="1">
-        <v>60</v>
+        <v>9</v>
+      </c>
+      <c r="F41" s="1">
+        <v>2</v>
       </c>
       <c r="G41" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="H41" s="1" t="s">
-        <v>140</v>
+        <v>69</v>
+      </c>
+      <c r="I41" s="1" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="42" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
-        <v>195</v>
+        <v>168</v>
       </c>
       <c r="B42" s="1">
         <v>2017</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>71</v>
+        <v>11</v>
       </c>
       <c r="E42" s="1">
+        <v>60</v>
+      </c>
+      <c r="G42" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="H42" s="1" t="s">
         <v>140</v>
-      </c>
-      <c r="F42" s="1">
-        <v>6</v>
-      </c>
-      <c r="G42" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="H42" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="I42" s="1" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="43" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B43" s="1">
         <v>2017</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="E43" s="1">
-        <v>10</v>
+        <v>140</v>
+      </c>
+      <c r="F43" s="1">
+        <v>6</v>
       </c>
       <c r="G43" s="4" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="H43" s="1" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="44" spans="1:9" ht="68" x14ac:dyDescent="0.2">
+        <v>141</v>
+      </c>
+      <c r="I43" s="1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B44" s="1">
         <v>2017</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>75</v>
+        <v>220</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>36</v>
+        <v>73</v>
       </c>
       <c r="E44" s="1">
-        <v>111</v>
-      </c>
-      <c r="F44" s="1">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="G44" s="4" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="H44" s="1" t="s">
-        <v>76</v>
+        <v>142</v>
       </c>
     </row>
     <row r="45" spans="1:9" ht="68" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B45" s="1">
         <v>2017</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>221</v>
+        <v>75</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>79</v>
+        <v>36</v>
       </c>
       <c r="E45" s="1">
-        <v>55</v>
+        <v>111</v>
+      </c>
+      <c r="F45" s="1">
+        <v>5</v>
       </c>
       <c r="G45" s="4" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="H45" s="1" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="46" spans="1:9" ht="51" x14ac:dyDescent="0.2">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" ht="68" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
-        <v>188</v>
+        <v>198</v>
       </c>
       <c r="B46" s="1">
         <v>2017</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>81</v>
+        <v>221</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="E46" s="1">
-        <v>36</v>
-      </c>
-      <c r="F46" s="1">
-        <v>6</v>
+        <v>55</v>
       </c>
       <c r="G46" s="4" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="H46" s="1" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
     </row>
     <row r="47" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
-        <v>168</v>
+        <v>188</v>
       </c>
       <c r="B47" s="1">
         <v>2017</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>11</v>
+        <v>82</v>
       </c>
       <c r="E47" s="1">
-        <v>60</v>
+        <v>36</v>
       </c>
       <c r="F47" s="1">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="G47" s="4" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="H47" s="1" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="48" spans="1:9" ht="34" x14ac:dyDescent="0.2">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
-        <v>199</v>
+        <v>168</v>
       </c>
       <c r="B48" s="1">
         <v>2017</v>
       </c>
       <c r="C48" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E48" s="1">
+        <v>60</v>
+      </c>
+      <c r="F48" s="1">
+        <v>3</v>
+      </c>
+      <c r="G48" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="H48" s="1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="A49" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="B49" s="1">
+        <v>2017</v>
+      </c>
+      <c r="C49" s="1" t="s">
         <v>222</v>
       </c>
-      <c r="D48" s="1" t="s">
+      <c r="D49" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="E48" s="1">
+      <c r="E49" s="1">
         <v>30</v>
-      </c>
-      <c r="F48" s="1">
-        <v>2</v>
-      </c>
-      <c r="G48" s="4" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="49" spans="1:7" ht="51" x14ac:dyDescent="0.2">
-      <c r="A49" s="1" t="s">
-        <v>195</v>
-      </c>
-      <c r="B49" s="1">
-        <v>2016</v>
-      </c>
-      <c r="C49" s="1" t="s">
-        <v>223</v>
-      </c>
-      <c r="D49" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="E49" s="1">
-        <v>1</v>
       </c>
       <c r="F49" s="1">
         <v>2</v>
       </c>
       <c r="G49" s="4" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="50" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" ht="51" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="B50" s="1">
         <v>2016</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="D50" s="1" t="s">
         <v>62</v>
@@ -2316,52 +2316,75 @@
         <v>2</v>
       </c>
       <c r="G50" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="51" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B51" s="1">
         <v>2016</v>
       </c>
       <c r="C51" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="D51" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="E51" s="1">
+        <v>1</v>
+      </c>
+      <c r="F51" s="1">
+        <v>2</v>
+      </c>
+      <c r="G51" s="4" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="A52" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="B52" s="1">
+        <v>2016</v>
+      </c>
+      <c r="C52" s="1" t="s">
         <v>225</v>
       </c>
-      <c r="D51" s="1" t="s">
+      <c r="D52" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="E51" s="1">
+      <c r="E52" s="1">
         <v>37</v>
       </c>
-      <c r="F51" s="1">
+      <c r="F52" s="1">
         <v>6</v>
       </c>
-      <c r="G51" s="4" t="s">
+      <c r="G52" s="4" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="52" spans="1:7" ht="68" x14ac:dyDescent="0.2">
-      <c r="A52" s="1" t="s">
+    <row r="53" spans="1:7" ht="68" x14ac:dyDescent="0.2">
+      <c r="A53" s="1" t="s">
         <v>202</v>
       </c>
-      <c r="B52" s="1">
+      <c r="B53" s="1">
         <v>2015</v>
       </c>
-      <c r="C52" s="1" t="s">
+      <c r="C53" s="1" t="s">
         <v>226</v>
       </c>
-      <c r="D52" s="1" t="s">
+      <c r="D53" s="1" t="s">
         <v>227</v>
       </c>
-      <c r="E52" s="1">
+      <c r="E53" s="1">
         <v>115</v>
       </c>
-      <c r="F52" s="1">
+      <c r="F53" s="1">
         <v>5</v>
       </c>
-      <c r="G52" s="4" t="s">
+      <c r="G53" s="4" t="s">
         <v>94</v>
       </c>
     </row>

</xml_diff>

<commit_message>
updated cv with grants in pubs
</commit_message>
<xml_diff>
--- a/assets/CV/pubs.xlsx
+++ b/assets/CV/pubs.xlsx
@@ -8,16 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tbarret/Dropbox/GitHub/blog_rstats/assets/CV/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C2A7184-1F43-5943-80E4-36B3C99B5FC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAD1EF66-612D-554A-87FF-F513A28778B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6300" yWindow="460" windowWidth="22500" windowHeight="16520" xr2:uid="{D694CAF4-E52C-7242-8187-CC366AD31369}"/>
+    <workbookView xWindow="4260" yWindow="460" windowWidth="24540" windowHeight="16520" activeTab="1" xr2:uid="{D694CAF4-E52C-7242-8187-CC366AD31369}"/>
   </bookViews>
   <sheets>
     <sheet name="Journals" sheetId="1" r:id="rId1"/>
-    <sheet name="Presentations" sheetId="2" r:id="rId2"/>
+    <sheet name="Grants" sheetId="3" r:id="rId2"/>
+    <sheet name="Presentations" sheetId="2" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_Hlk70254864" localSheetId="0">Journals!$A$18</definedName>
+    <definedName name="_Hlk70254864" localSheetId="0">Journals!$A$20</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="349" uniqueCount="313">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="437" uniqueCount="387">
   <si>
     <t>authors</t>
   </si>
@@ -367,9 +368,6 @@
     <t>\hyperlink{https://www.medrxiv.org/content/10.1101/2020.07.22.20158949v1}{medRxiv Pre-Print}</t>
   </si>
   <si>
-    <t>1-11</t>
-  </si>
-  <si>
     <t>doi: 10.1002/jclp.23162</t>
   </si>
   <si>
@@ -379,9 +377,6 @@
     <t>doi: 10.1080/09687637.2021.1936457</t>
   </si>
   <si>
-    <t> 68</t>
-  </si>
-  <si>
     <t>49-55</t>
   </si>
   <si>
@@ -826,9 +821,6 @@
     <t xml:space="preserve">doi: 10.1044/2021_JSLHR-20-00663 </t>
   </si>
   <si>
-    <t>1-15</t>
-  </si>
-  <si>
     <t>Chronic health conditions and adolescent friendships: Perspectives from social network analysis.</t>
   </si>
   <si>
@@ -865,12 +857,6 @@
     <t>doi: 10.1044/2022_AJSLP-22-00003</t>
   </si>
   <si>
-    <t>1-18</t>
-  </si>
-  <si>
-    <t>1-14</t>
-  </si>
-  <si>
     <t>Tannahill, H. S., Barrett, T. S., Zalta, A. K., Tehee, M., &amp; Blais, R. K.</t>
   </si>
   <si>
@@ -961,9 +947,6 @@
     <t>doi: 10.1080/26924951.2023.2200987</t>
   </si>
   <si>
-    <t xml:space="preserve"> La vergüenza [the shame]: Meassuring affiliate stigma associated with youth mental health problems among Latinx caregivers.</t>
-  </si>
-  <si>
     <t>Vázquez, A. L., Domenech Rodríguez, M. M., Navarro Flores, C. M.,  Abreu, R. L., &amp; Barrett, T. S.</t>
   </si>
   <si>
@@ -977,13 +960,256 @@
   </si>
   <si>
     <t>Yoho, S. E., Barrett, T. S., &amp; Borrie, S. A.</t>
+  </si>
+  <si>
+    <t>Perceptual learning of dysarthria in adolescence</t>
+  </si>
+  <si>
+    <t>Borrie, S. A., Hepworth, T. J., Wynn, C. J., Hustad, K. C.,  Barrett, T. S., &amp; Lansford, K. L.</t>
+  </si>
+  <si>
+    <t>Voss, M. W., Barrett, T. S., Campbell, A. &amp; Van Komen, A.</t>
+  </si>
+  <si>
+    <t>Parenting and the opioid epidemic: A systematic scoping review.</t>
+  </si>
+  <si>
+    <t>1280-1293</t>
+  </si>
+  <si>
+    <t>Journal of Child and Family Studies</t>
+  </si>
+  <si>
+    <t>30-47</t>
+  </si>
+  <si>
+    <t>e2895</t>
+  </si>
+  <si>
+    <t xml:space="preserve">doi: 10.1002/brb3.2895 </t>
+  </si>
+  <si>
+    <t>doi: 10.1044/2023_JSLHR-22-00263</t>
+  </si>
+  <si>
+    <t>doi: 10.1007/s10826-023-02576-2</t>
+  </si>
+  <si>
+    <t>1853-1866</t>
+  </si>
+  <si>
+    <t>doi: 10.1044/2023_JSLHR-22-00558</t>
+  </si>
+  <si>
+    <t>\img{osfdata.png}{https://osf.io/z6dw5}\img{osfmaterials.png}{https://osf.io/z6dw5}</t>
+  </si>
+  <si>
+    <t>La vergüenza [the shame]: Meassuring affiliate stigma associated with youth mental health problems among Latinx caregivers.</t>
+  </si>
+  <si>
+    <t>2187-2203</t>
+  </si>
+  <si>
+    <t>doi: 10.1044/2022_JSLHR-21-00293</t>
+  </si>
+  <si>
+    <t>doi: 10.1080/10640266.2022.2141710</t>
+  </si>
+  <si>
+    <t>388-404</t>
+  </si>
+  <si>
+    <t>576-586</t>
+  </si>
+  <si>
+    <t>\img{osfdata.png}{https://osf.io/vygeh/}\img{osfmaterials.png}{https://osf.io/vygeh/}</t>
+  </si>
+  <si>
+    <t>958–972</t>
+  </si>
+  <si>
+    <t>722-738</t>
+  </si>
+  <si>
+    <t>847–864</t>
+  </si>
+  <si>
+    <t>2181-2192</t>
+  </si>
+  <si>
+    <t>1501-1510</t>
+  </si>
+  <si>
+    <t>1208-1215</t>
+  </si>
+  <si>
+    <t>2004-2021</t>
+  </si>
+  <si>
+    <t>314-322</t>
+  </si>
+  <si>
+    <t>doi: 10.1016/j.jsr.2022.06.007</t>
+  </si>
+  <si>
+    <t>217</t>
+  </si>
+  <si>
+    <t>doi: 10.1038/s41398-022-01967-1</t>
+  </si>
+  <si>
+    <t>\img{osfmaterials.png}{https://osf.io/csgmf/}</t>
+  </si>
+  <si>
+    <t>doi: 10.1044/2022_JSLHR-22-00391</t>
+  </si>
+  <si>
+    <t>doi: 10.1080/00140139.2022.2141347</t>
+  </si>
+  <si>
+    <t>doi: 10.3758/s13414-018-1635-3</t>
+  </si>
+  <si>
+    <t>doi: 10.1044/2018_JSLHR-S-18-0210</t>
+  </si>
+  <si>
+    <t>doi: 10.26077/egtr-0805</t>
+  </si>
+  <si>
+    <t>doi: 10.1097/IYC.0000000000000090</t>
+  </si>
+  <si>
+    <t>doi: 10.15142/T3P88B</t>
+  </si>
+  <si>
+    <t>doi: 10.15142/T32G62</t>
+  </si>
+  <si>
+    <t>doi: 10.1097/AUD.0000000000000338</t>
+  </si>
+  <si>
+    <t>doi: 10.1016/j.jand.2014.10.015</t>
+  </si>
+  <si>
+    <t>funder</t>
+  </si>
+  <si>
+    <t>status</t>
+  </si>
+  <si>
+    <t>amount</t>
+  </si>
+  <si>
+    <t>A causal framework of communicative participation in people with Parkinson's disease</t>
+  </si>
+  <si>
+    <t>Borrie, S. A. (PI), Barrett, T. S. (Co-I), Visar, B. (Co-I), &amp; Liss, J. (Co-I)</t>
+  </si>
+  <si>
+    <t>NIH/NIDCD</t>
+  </si>
+  <si>
+    <t>R01DC020713-01A1</t>
+  </si>
+  <si>
+    <t>number</t>
+  </si>
+  <si>
+    <t>Funded</t>
+  </si>
+  <si>
+    <t>type</t>
+  </si>
+  <si>
+    <t>NIH R01</t>
+  </si>
+  <si>
+    <t>Speaker and listener strategies to improve intelligibility in Parkinson's disease</t>
+  </si>
+  <si>
+    <t>Lansford, K. L. (PI), Borrie, S. A. (Co-I), &amp; Barrett, T. S. (Co-I)</t>
+  </si>
+  <si>
+    <t>Parkinson's Foundation</t>
+  </si>
+  <si>
+    <t>Necessary Education and eXperiential Training for Upcoming Para-professionals (NEXT-UP)</t>
+  </si>
+  <si>
+    <t>Voss, M. (PI) &amp; Barrett, T. S. (Co-I)</t>
+  </si>
+  <si>
+    <t>HRSA</t>
+  </si>
+  <si>
+    <t>1 T26HP39463-01-00</t>
+  </si>
+  <si>
+    <t>Video- and App-Based Naturalistic Language Instruction (VALI) for Spanish-Speaking Caregivers to Support Bilingual Language Development in Children With or At Risk for Language Delays</t>
+  </si>
+  <si>
+    <t>Larson, A. (PI), Snyder, P. (Mentor) Domenech Rodriguez, M. (Mentor), &amp; Barrett, T. S. (Consultant)</t>
+  </si>
+  <si>
+    <t>IES/NCSER</t>
+  </si>
+  <si>
+    <t>R324B200009</t>
+  </si>
+  <si>
+    <t>IES</t>
+  </si>
+  <si>
+    <t>Bridging Harm Reduction and Wellness for Tribal and Rural Areas of the Intermountain West</t>
+  </si>
+  <si>
+    <t>Sulzer, S. (PI), Prevedel, S., Chapoose, M., Madden, E., Barrett, T. S. (Co-I), Keady, T., Peatross, J., DasGupta, D., Fullenkamp, N., &amp; Zaman, K</t>
+  </si>
+  <si>
+    <t>H79TI083267</t>
+  </si>
+  <si>
+    <t>SAMHSA</t>
+  </si>
+  <si>
+    <t>Application of Ideal Binary Masking to Disordered Speech</t>
+  </si>
+  <si>
+    <t>Leopold, S. (PI), Borrie, S. A. (Co-I), &amp; Barrett, T. S. (Co-I)</t>
+  </si>
+  <si>
+    <t>1R21DC018641-01</t>
+  </si>
+  <si>
+    <t>Completed</t>
+  </si>
+  <si>
+    <t>NIH R21</t>
+  </si>
+  <si>
+    <t>Perceptual training for improved intelligibility of dysarthric speech</t>
+  </si>
+  <si>
+    <t>Borrie, S. A. (PI), Lansford, K. (PI), &amp; Barrett, T. S. (Co-I)</t>
+  </si>
+  <si>
+    <t>1R21DC018867-01</t>
+  </si>
+  <si>
+    <t>start</t>
+  </si>
+  <si>
+    <t>end</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5">
+  <numFmts count="1">
+    <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
+  </numFmts>
+  <fonts count="9">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1016,6 +1242,31 @@
       <color theme="1"/>
       <name val="AdvOT1ef757c0"/>
     </font>
+    <font>
+      <sz val="13"/>
+      <color rgb="FF222222"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF222222"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF211E1E"/>
+      <name val="AdvTTf0797824"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -1040,10 +1291,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1065,8 +1317,19 @@
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1379,10 +1642,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38BAB23D-B27F-A34D-A522-4C115B575C05}">
-  <dimension ref="A1:I72"/>
+  <dimension ref="A1:I74"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1428,15 +1691,15 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="51">
+    <row r="2" spans="1:9" ht="34">
       <c r="A2" s="1" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>302</v>
+        <v>297</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>11</v>
@@ -1445,497 +1708,614 @@
     </row>
     <row r="3" spans="1:9" ht="51">
       <c r="A3" s="1" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>297</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>305</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G3" s="1"/>
+    </row>
+    <row r="4" spans="1:9" ht="51">
+      <c r="A4" s="1" t="s">
         <v>302</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>307</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>309</v>
-      </c>
-      <c r="G3" s="1"/>
-    </row>
-    <row r="4" spans="1:9" ht="68">
-      <c r="A4" s="1" t="s">
+      <c r="B4" s="1" t="s">
+        <v>297</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>321</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>303</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>302</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>304</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>305</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" ht="51">
+      <c r="G4" s="1"/>
+    </row>
+    <row r="5" spans="1:9" ht="68">
       <c r="A5" s="1" t="s">
-        <v>296</v>
-      </c>
-      <c r="B5" s="1">
-        <v>2023</v>
+        <v>298</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>297</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>297</v>
+        <v>299</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" ht="34">
-      <c r="A6" s="5" t="s">
-        <v>292</v>
+        <v>300</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>301</v>
+      </c>
+      <c r="I5" s="11"/>
+    </row>
+    <row r="6" spans="1:9" ht="68">
+      <c r="A6" s="1" t="s">
+        <v>272</v>
       </c>
       <c r="B6" s="1">
         <v>2023</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>293</v>
+        <v>273</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>11</v>
+        <v>264</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="51">
       <c r="A7" s="1" t="s">
-        <v>291</v>
+        <v>268</v>
       </c>
       <c r="B7" s="1">
         <v>2023</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>294</v>
+        <v>269</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" ht="68">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="51">
       <c r="A8" s="1" t="s">
-        <v>277</v>
+        <v>291</v>
       </c>
       <c r="B8" s="1">
         <v>2023</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>278</v>
+        <v>292</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>267</v>
+        <v>11</v>
+      </c>
+      <c r="E8" s="1">
+        <v>66</v>
+      </c>
+      <c r="F8" s="1">
+        <v>5</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>318</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>319</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>320</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="51">
       <c r="A9" s="1" t="s">
-        <v>271</v>
+        <v>309</v>
       </c>
       <c r="B9" s="1">
         <v>2023</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>272</v>
+        <v>310</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" ht="68">
+        <v>312</v>
+      </c>
+      <c r="E9" s="1">
+        <v>32</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>311</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="51">
       <c r="A10" s="5" t="s">
-        <v>249</v>
+        <v>287</v>
       </c>
       <c r="B10" s="1">
         <v>2023</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>250</v>
+        <v>288</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="E10" s="1">
-        <v>62</v>
-      </c>
-      <c r="F10" s="1">
-        <v>5</v>
-      </c>
-      <c r="G10" s="4" t="s">
-        <v>310</v>
+        <v>11</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>252</v>
-      </c>
-      <c r="I10" s="1" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" ht="68">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="51">
       <c r="A11" s="1" t="s">
-        <v>298</v>
+        <v>286</v>
       </c>
       <c r="B11" s="1">
         <v>2023</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>299</v>
+        <v>289</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>267</v>
+        <v>285</v>
       </c>
       <c r="E11" s="1">
+        <v>13</v>
+      </c>
+      <c r="F11" s="1">
+        <v>2</v>
+      </c>
+      <c r="G11" s="9" t="s">
+        <v>314</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="68">
+      <c r="A12" s="5" t="s">
+        <v>247</v>
+      </c>
+      <c r="B12" s="1">
+        <v>2023</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="E12" s="1">
+        <v>62</v>
+      </c>
+      <c r="F12" s="1">
+        <v>5</v>
+      </c>
+      <c r="G12" s="4" t="s">
+        <v>304</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="68">
+      <c r="A13" s="1" t="s">
+        <v>293</v>
+      </c>
+      <c r="B13" s="1">
+        <v>2023</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>294</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="E13" s="1">
         <v>38</v>
       </c>
-      <c r="F11" s="8">
+      <c r="F13" s="8">
         <v>44989</v>
       </c>
-      <c r="G11" s="4" t="s">
-        <v>300</v>
-      </c>
-      <c r="H11" s="1" t="s">
-        <v>301</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" ht="34">
-      <c r="A12" s="1" t="s">
-        <v>279</v>
-      </c>
-      <c r="B12" s="1">
-        <v>2022</v>
-      </c>
-      <c r="C12" s="1" t="s">
+      <c r="G13" s="4" t="s">
         <v>295</v>
       </c>
-      <c r="D12" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" ht="34">
-      <c r="A13" s="1" t="s">
-        <v>287</v>
-      </c>
-      <c r="B13" s="1">
-        <v>2022</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>288</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>289</v>
+      <c r="H13" s="1" t="s">
+        <v>296</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="51">
       <c r="A14" s="1" t="s">
-        <v>280</v>
+        <v>274</v>
       </c>
       <c r="B14" s="1">
         <v>2022</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>281</v>
+        <v>290</v>
       </c>
       <c r="D14" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E14" s="1">
+        <v>66</v>
+      </c>
+      <c r="F14" s="1">
+        <v>1</v>
+      </c>
+      <c r="G14" s="10" t="s">
+        <v>313</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="68">
+      <c r="A15" s="1" t="s">
         <v>282</v>
-      </c>
-      <c r="E14" s="1">
-        <v>26</v>
-      </c>
-      <c r="G14" s="4" t="s">
-        <v>283</v>
-      </c>
-      <c r="H14" s="1" t="s">
-        <v>284</v>
-      </c>
-      <c r="I14" s="1" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" ht="51">
-      <c r="A15" s="1" t="s">
-        <v>266</v>
       </c>
       <c r="B15" s="1">
         <v>2022</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>265</v>
-      </c>
-      <c r="E15" s="1">
-        <v>12</v>
-      </c>
-      <c r="F15" s="1">
-        <v>1</v>
+        <v>284</v>
       </c>
       <c r="G15" s="4" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" ht="34">
-      <c r="A16" s="5" t="s">
-        <v>251</v>
+        <v>85</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>341</v>
+      </c>
+      <c r="I15" s="12"/>
+    </row>
+    <row r="16" spans="1:9" ht="51">
+      <c r="A16" s="1" t="s">
+        <v>275</v>
       </c>
       <c r="B16" s="1">
         <v>2022</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>269</v>
+        <v>276</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>11</v>
+        <v>277</v>
+      </c>
+      <c r="E16" s="1">
+        <v>26</v>
       </c>
       <c r="G16" s="4" t="s">
-        <v>212</v>
+        <v>278</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>279</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>237</v>
+        <v>281</v>
       </c>
     </row>
     <row r="17" spans="1:9" ht="51">
-      <c r="A17" s="5" t="s">
-        <v>230</v>
+      <c r="A17" s="1" t="s">
+        <v>263</v>
       </c>
       <c r="B17" s="1">
         <v>2022</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>228</v>
+        <v>280</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>229</v>
+        <v>262</v>
+      </c>
+      <c r="E17" s="1">
+        <v>12</v>
       </c>
       <c r="G17" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="I17" s="7"/>
-    </row>
-    <row r="18" spans="1:9" ht="34">
-      <c r="A18" s="6" t="s">
-        <v>243</v>
+        <v>337</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>338</v>
+      </c>
+      <c r="I17" s="1" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="51">
+      <c r="A18" s="5" t="s">
+        <v>249</v>
       </c>
       <c r="B18" s="1">
         <v>2022</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>245</v>
+        <v>266</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" ht="51">
-      <c r="A19" s="1" t="s">
-        <v>268</v>
+        <v>11</v>
+      </c>
+      <c r="E18" s="1">
+        <v>65</v>
+      </c>
+      <c r="F18" s="1">
+        <v>6</v>
+      </c>
+      <c r="G18" s="4" t="s">
+        <v>322</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>323</v>
+      </c>
+      <c r="I18" s="1" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="68">
+      <c r="A19" s="5" t="s">
+        <v>228</v>
       </c>
       <c r="B19" s="1">
         <v>2022</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>270</v>
+        <v>226</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>147</v>
+        <v>227</v>
+      </c>
+      <c r="E19" s="1">
+        <v>31</v>
+      </c>
+      <c r="F19" s="1">
+        <v>4</v>
       </c>
       <c r="G19" s="4" t="s">
-        <v>275</v>
+        <v>325</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>274</v>
-      </c>
+        <v>324</v>
+      </c>
+      <c r="I19" s="7"/>
     </row>
     <row r="20" spans="1:9" ht="51">
-      <c r="A20" s="5" t="s">
+      <c r="A20" s="6" t="s">
         <v>241</v>
       </c>
       <c r="B20" s="1">
         <v>2022</v>
       </c>
       <c r="C20" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="D20" s="1" t="s">
         <v>244</v>
       </c>
-      <c r="D20" s="1" t="s">
-        <v>34</v>
+      <c r="E20" s="1">
+        <v>82</v>
+      </c>
+      <c r="G20" s="4" t="s">
+        <v>335</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>254</v>
-      </c>
-      <c r="I20" s="1" t="s">
-        <v>242</v>
+        <v>336</v>
       </c>
     </row>
     <row r="21" spans="1:9" ht="51">
-      <c r="A21" s="5" t="s">
-        <v>236</v>
+      <c r="A21" s="1" t="s">
+        <v>265</v>
       </c>
       <c r="B21" s="1">
         <v>2022</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>234</v>
+        <v>267</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>235</v>
+        <v>145</v>
+      </c>
+      <c r="E21" s="1">
+        <v>31</v>
+      </c>
+      <c r="F21" s="1">
+        <v>5</v>
+      </c>
+      <c r="G21" s="4" t="s">
+        <v>334</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>248</v>
-      </c>
-      <c r="I21" s="1" t="s">
-        <v>239</v>
+        <v>271</v>
       </c>
     </row>
     <row r="22" spans="1:9" ht="51">
       <c r="A22" s="5" t="s">
-        <v>231</v>
+        <v>239</v>
       </c>
       <c r="B22" s="1">
         <v>2022</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>232</v>
+        <v>242</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>233</v>
+        <v>34</v>
+      </c>
+      <c r="E22" s="1">
+        <v>23</v>
+      </c>
+      <c r="F22" s="1">
+        <v>7</v>
+      </c>
+      <c r="G22" s="4" t="s">
+        <v>333</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>247</v>
+        <v>252</v>
+      </c>
+      <c r="I22" s="1" t="s">
+        <v>240</v>
       </c>
     </row>
     <row r="23" spans="1:9" ht="51">
-      <c r="A23" s="1" t="s">
-        <v>155</v>
+      <c r="A23" s="5" t="s">
+        <v>234</v>
       </c>
       <c r="B23" s="1">
         <v>2022</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>227</v>
+        <v>232</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>150</v>
+        <v>233</v>
+      </c>
+      <c r="E23" s="1">
+        <v>37</v>
+      </c>
+      <c r="F23" s="1">
+        <v>6</v>
+      </c>
+      <c r="G23" s="4" t="s">
+        <v>332</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" ht="68">
-      <c r="A24" s="1" t="s">
-        <v>157</v>
+        <v>246</v>
+      </c>
+      <c r="I23" s="1" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" ht="51">
+      <c r="A24" s="5" t="s">
+        <v>229</v>
       </c>
       <c r="B24" s="1">
         <v>2022</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>148</v>
+        <v>230</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>147</v>
+        <v>231</v>
+      </c>
+      <c r="E24" s="1">
+        <v>27</v>
+      </c>
+      <c r="F24" s="1">
+        <v>6</v>
       </c>
       <c r="G24" s="4" t="s">
-        <v>212</v>
+        <v>331</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>240</v>
+        <v>245</v>
       </c>
     </row>
     <row r="25" spans="1:9" ht="51">
       <c r="A25" s="1" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="B25" s="1">
         <v>2022</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>149</v>
+        <v>225</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>11</v>
+        <v>148</v>
       </c>
       <c r="E25" s="1">
-        <v>65</v>
-      </c>
-      <c r="F25" s="1">
-        <v>2</v>
+        <v>51</v>
       </c>
       <c r="G25" s="4" t="s">
-        <v>264</v>
+        <v>330</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>238</v>
-      </c>
-      <c r="I25" s="1" t="s">
-        <v>237</v>
+        <v>152</v>
       </c>
     </row>
     <row r="26" spans="1:9" ht="68">
       <c r="A26" s="1" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="B26" s="1">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="E26" s="1">
-        <v>131</v>
+        <v>31</v>
+      </c>
+      <c r="F26" s="1">
+        <v>2</v>
       </c>
       <c r="G26" s="4" t="s">
-        <v>226</v>
+        <v>329</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>153</v>
+        <v>238</v>
       </c>
     </row>
     <row r="27" spans="1:9" ht="51">
       <c r="A27" s="1" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="B27" s="1">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>200</v>
+        <v>147</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>141</v>
+        <v>11</v>
+      </c>
+      <c r="E27" s="1">
+        <v>65</v>
+      </c>
+      <c r="F27" s="1">
+        <v>2</v>
       </c>
       <c r="G27" s="4" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>225</v>
+        <v>236</v>
+      </c>
+      <c r="I27" s="1" t="s">
+        <v>235</v>
       </c>
     </row>
     <row r="28" spans="1:9" ht="68">
       <c r="A28" s="1" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="B28" s="1">
         <v>2021</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="E28">
-        <v>16</v>
-      </c>
-      <c r="F28" s="1">
-        <v>10</v>
+        <v>142</v>
+      </c>
+      <c r="E28" s="1">
+        <v>131</v>
       </c>
       <c r="G28" s="4" t="s">
-        <v>152</v>
+        <v>224</v>
       </c>
       <c r="H28" s="1" t="s">
         <v>151</v>
@@ -1943,192 +2323,199 @@
     </row>
     <row r="29" spans="1:9" ht="51">
       <c r="A29" s="1" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="B29" s="1">
         <v>2021</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>5</v>
+        <v>198</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>6</v>
+        <v>139</v>
       </c>
       <c r="E29" s="1">
-        <v>38</v>
+        <v>21</v>
       </c>
       <c r="G29" s="4" t="s">
-        <v>117</v>
+        <v>328</v>
       </c>
       <c r="H29" s="1" t="s">
-        <v>116</v>
+        <v>223</v>
       </c>
     </row>
     <row r="30" spans="1:9" ht="68">
       <c r="A30" s="1" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="B30" s="1">
         <v>2021</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>201</v>
+        <v>144</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>111</v>
+        <v>143</v>
+      </c>
+      <c r="E30">
+        <v>16</v>
+      </c>
+      <c r="F30" s="1">
+        <v>10</v>
       </c>
       <c r="G30" s="4" t="s">
-        <v>109</v>
+        <v>150</v>
       </c>
       <c r="H30" s="1" t="s">
-        <v>112</v>
+        <v>149</v>
       </c>
     </row>
     <row r="31" spans="1:9" ht="51">
       <c r="A31" s="1" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="B31" s="1">
         <v>2021</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E31" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="F31" s="1">
-        <v>1</v>
+        <v>6</v>
+      </c>
+      <c r="E31" s="1">
+        <v>38</v>
       </c>
       <c r="G31" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="H31" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="H31" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="I31" s="1" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" ht="51">
+      <c r="I31" s="12"/>
+    </row>
+    <row r="32" spans="1:9" ht="68">
       <c r="A32" s="1" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="B32" s="1">
         <v>2021</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>9</v>
+        <v>199</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>10</v>
+        <v>110</v>
       </c>
       <c r="E32" s="1">
-        <v>77</v>
+        <v>29</v>
       </c>
       <c r="F32" s="1">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="G32" s="4" t="s">
-        <v>142</v>
+        <v>326</v>
       </c>
       <c r="H32" s="1" t="s">
-        <v>110</v>
+        <v>111</v>
+      </c>
+      <c r="I32" s="1" t="s">
+        <v>327</v>
       </c>
     </row>
     <row r="33" spans="1:9" ht="51">
       <c r="A33" s="1" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="B33" s="1">
         <v>2021</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>202</v>
+        <v>7</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="E33" s="1">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="F33" s="1">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="G33" s="4" t="s">
-        <v>260</v>
+        <v>112</v>
       </c>
       <c r="H33" s="1" t="s">
-        <v>261</v>
+        <v>113</v>
       </c>
       <c r="I33" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="34" spans="1:9" ht="51">
       <c r="A34" s="1" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="B34" s="1">
         <v>2021</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E34" s="1">
-        <v>64</v>
+        <v>77</v>
       </c>
       <c r="F34" s="1">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="G34" s="4" t="s">
-        <v>258</v>
+        <v>140</v>
       </c>
       <c r="H34" s="1" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9" ht="68">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" ht="51">
       <c r="A35" s="1" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="B35" s="1">
         <v>2021</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>94</v>
+        <v>11</v>
       </c>
       <c r="E35" s="1">
-        <v>60</v>
+        <v>64</v>
+      </c>
+      <c r="F35" s="1">
+        <v>5</v>
       </c>
       <c r="G35" s="4" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="H35" s="1" t="s">
-        <v>118</v>
+        <v>259</v>
       </c>
       <c r="I35" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="36" spans="1:9" ht="51">
       <c r="A36" s="1" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="B36" s="1">
         <v>2021</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>204</v>
+        <v>12</v>
       </c>
       <c r="D36" s="1" t="s">
         <v>11</v>
@@ -2137,206 +2524,203 @@
         <v>64</v>
       </c>
       <c r="F36" s="1">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="G36" s="4" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="H36" s="1" t="s">
-        <v>119</v>
+        <v>257</v>
       </c>
     </row>
     <row r="37" spans="1:9" ht="68">
       <c r="A37" s="1" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="B37" s="1">
         <v>2021</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>13</v>
+        <v>94</v>
       </c>
       <c r="E37" s="1">
-        <v>23</v>
-      </c>
-      <c r="F37" s="1">
-        <v>5</v>
+        <v>60</v>
       </c>
       <c r="G37" s="4" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="H37" s="1" t="s">
-        <v>16</v>
+        <v>116</v>
       </c>
       <c r="I37" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="38" spans="1:9" ht="51">
       <c r="A38" s="1" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="B38" s="1">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>14</v>
+        <v>202</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="E38" s="1">
-        <v>42</v>
+        <v>64</v>
+      </c>
+      <c r="F38" s="1">
+        <v>2</v>
       </c>
       <c r="G38" s="4" t="s">
-        <v>20</v>
+        <v>253</v>
       </c>
       <c r="H38" s="1" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="39" spans="1:9" ht="51">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" ht="68">
       <c r="A39" s="1" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="B39" s="1">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>22</v>
+        <v>203</v>
       </c>
       <c r="D39" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E39" s="1">
         <v>23</v>
       </c>
-      <c r="E39" s="1">
-        <v>18</v>
+      <c r="F39" s="1">
+        <v>5</v>
       </c>
       <c r="G39" s="4" t="s">
-        <v>24</v>
+        <v>254</v>
       </c>
       <c r="H39" s="1" t="s">
-        <v>121</v>
+        <v>16</v>
+      </c>
+      <c r="I39" s="1" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="40" spans="1:9" ht="51">
       <c r="A40" s="1" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="B40" s="1">
         <v>2020</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="E40" s="1">
-        <v>63</v>
-      </c>
-      <c r="F40" s="1">
-        <v>6</v>
+        <v>42</v>
       </c>
       <c r="G40" s="4" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="H40" s="1" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
     </row>
     <row r="41" spans="1:9" ht="51">
       <c r="A41" s="1" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="B41" s="1">
         <v>2020</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>206</v>
+        <v>22</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="E41" s="1">
-        <v>40</v>
+        <v>18</v>
       </c>
       <c r="G41" s="4" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="H41" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="I41" s="1" t="s">
-        <v>108</v>
+        <v>119</v>
       </c>
     </row>
     <row r="42" spans="1:9" ht="51">
       <c r="A42" s="1" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="B42" s="1">
         <v>2020</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>207</v>
+        <v>25</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="E42" s="1">
-        <v>51</v>
+        <v>63</v>
       </c>
       <c r="F42" s="1">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="G42" s="4" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H42" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="I42" s="1" t="s">
-        <v>99</v>
+        <v>120</v>
       </c>
     </row>
     <row r="43" spans="1:9" ht="51">
       <c r="A43" s="1" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="B43" s="1">
         <v>2020</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>31</v>
+        <v>204</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>11</v>
+        <v>27</v>
       </c>
       <c r="E43" s="1">
-        <v>63</v>
-      </c>
-      <c r="F43" s="1">
-        <v>8</v>
+        <v>40</v>
       </c>
       <c r="G43" s="4" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="H43" s="1" t="s">
-        <v>125</v>
+        <v>121</v>
+      </c>
+      <c r="I43" s="1" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="44" spans="1:9" ht="51">
       <c r="A44" s="1" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="B44" s="1">
         <v>2020</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="D44" s="1" t="s">
         <v>29</v>
@@ -2348,714 +2732,793 @@
         <v>3</v>
       </c>
       <c r="G44" s="4" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="H44" s="1" t="s">
-        <v>126</v>
+        <v>122</v>
+      </c>
+      <c r="I44" s="1" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="45" spans="1:9" ht="51">
       <c r="A45" s="1" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="B45" s="1">
         <v>2020</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>209</v>
+        <v>31</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>34</v>
+        <v>11</v>
       </c>
       <c r="E45" s="1">
-        <v>21</v>
+        <v>63</v>
       </c>
       <c r="F45" s="1">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="G45" s="4" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="H45" s="1" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="46" spans="1:9" ht="68">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" ht="51">
       <c r="A46" s="1" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="B46" s="1">
         <v>2020</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="E46" s="1">
-        <v>113</v>
+        <v>51</v>
       </c>
       <c r="F46" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G46" s="4" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="H46" s="1" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
     </row>
     <row r="47" spans="1:9" ht="51">
       <c r="A47" s="1" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="B47" s="1">
-        <v>2019</v>
+        <v>2020</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>38</v>
+        <v>207</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="E47" s="1">
-        <v>61</v>
+        <v>21</v>
       </c>
       <c r="F47" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G47" s="4" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="H47" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="I47" s="1" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="48" spans="1:9" ht="51">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" ht="68">
       <c r="A48" s="1" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B48" s="1">
-        <v>2019</v>
+        <v>2020</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>41</v>
+        <v>208</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>11</v>
+        <v>36</v>
       </c>
       <c r="E48" s="1">
-        <v>62</v>
+        <v>113</v>
       </c>
       <c r="F48" s="1">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="G48" s="4" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="H48" s="1" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
     </row>
     <row r="49" spans="1:9" ht="51">
       <c r="A49" s="1" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="B49" s="1">
         <v>2019</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="E49" s="1">
-        <v>10</v>
+        <v>61</v>
       </c>
       <c r="F49" s="1">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="G49" s="4" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="H49" s="1" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="I49" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="50" spans="1:9" ht="51">
       <c r="A50" s="1" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="B50" s="1">
         <v>2019</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="E50" s="1">
-        <v>13</v>
+        <v>62</v>
+      </c>
+      <c r="F50" s="1">
+        <v>12</v>
       </c>
       <c r="G50" s="4" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="H50" s="1" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
     </row>
     <row r="51" spans="1:9" ht="51">
       <c r="A51" s="1" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="B51" s="1">
         <v>2019</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="E51" s="1">
-        <v>22</v>
+        <v>10</v>
+      </c>
+      <c r="F51" s="1">
+        <v>10</v>
       </c>
       <c r="G51" s="4" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="H51" s="1" t="s">
-        <v>132</v>
+        <v>129</v>
+      </c>
+      <c r="I51" s="1" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="52" spans="1:9" ht="51">
       <c r="A52" s="1" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="B52" s="1">
         <v>2019</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>211</v>
+        <v>46</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>34</v>
+        <v>23</v>
       </c>
       <c r="E52" s="1">
-        <v>20</v>
-      </c>
-      <c r="F52" s="1">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="G52" s="4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="H52" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="I52" s="1" t="s">
-        <v>102</v>
+        <v>132</v>
       </c>
     </row>
     <row r="53" spans="1:9" ht="51">
       <c r="A53" s="1" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="B53" s="1">
         <v>2019</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>263</v>
+        <v>47</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="E53" s="1">
-        <v>33</v>
-      </c>
-      <c r="F53" s="1">
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="G53" s="4" t="s">
-        <v>212</v>
+        <v>50</v>
       </c>
       <c r="H53" s="1" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
     </row>
     <row r="54" spans="1:9" ht="51">
       <c r="A54" s="1" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="B54" s="1">
         <v>2019</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>53</v>
+        <v>209</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="E54" s="1">
-        <v>145</v>
+        <v>20</v>
       </c>
       <c r="F54" s="1">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G54" s="4" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="H54" s="1" t="s">
-        <v>55</v>
+        <v>131</v>
       </c>
       <c r="I54" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="55" spans="1:9" ht="51">
       <c r="A55" s="1" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="B55" s="1">
         <v>2019</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>58</v>
+        <v>260</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="E55" s="1">
-        <v>81</v>
+        <v>33</v>
       </c>
       <c r="F55" s="1">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="G55" s="4" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="56" spans="1:9" ht="68">
+        <v>210</v>
+      </c>
+      <c r="H55" s="1" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" ht="51">
       <c r="A56" s="1" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="B56" s="1">
         <v>2019</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>11</v>
+        <v>39</v>
       </c>
       <c r="E56" s="1">
-        <v>62</v>
+        <v>145</v>
       </c>
       <c r="F56" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G56" s="4" t="s">
-        <v>60</v>
+        <v>54</v>
+      </c>
+      <c r="H56" s="1" t="s">
+        <v>55</v>
       </c>
       <c r="I56" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="57" spans="1:9" ht="51">
       <c r="A57" s="1" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="B57" s="1">
-        <v>2018</v>
+        <v>2019</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>213</v>
+        <v>58</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="E57" s="1">
-        <v>3</v>
+        <v>81</v>
       </c>
       <c r="F57" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G57" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="H57" s="1" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" ht="68">
+      <c r="A58" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="B58" s="1">
+        <v>2019</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D58" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E58" s="1">
         <v>62</v>
       </c>
-      <c r="I57" s="1" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="58" spans="1:9" ht="51">
-      <c r="A58" s="1" t="s">
-        <v>190</v>
-      </c>
-      <c r="B58" s="1">
-        <v>2018</v>
-      </c>
-      <c r="C58" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="D58" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="E58" s="1">
-        <v>143</v>
-      </c>
       <c r="F58" s="1">
-        <v>3</v>
+        <v>2</v>
+      </c>
+      <c r="G58" s="4" t="s">
+        <v>60</v>
       </c>
       <c r="H58" s="1" t="s">
-        <v>136</v>
+        <v>343</v>
+      </c>
+      <c r="I58" s="1" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="59" spans="1:9" ht="51">
       <c r="A59" s="1" t="s">
-        <v>165</v>
+        <v>187</v>
       </c>
       <c r="B59" s="1">
         <v>2018</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>65</v>
+        <v>211</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="E59" s="1">
+        <v>3</v>
+      </c>
+      <c r="F59" s="1">
+        <v>1</v>
+      </c>
+      <c r="G59" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="H59" s="1" t="s">
+        <v>344</v>
+      </c>
+      <c r="I59" s="1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" ht="51">
+      <c r="A60" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="B60" s="1">
+        <v>2018</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="D60" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="E60" s="1">
         <v>143</v>
       </c>
-      <c r="F59" s="1">
-        <v>5</v>
-      </c>
-      <c r="H59" s="1" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="60" spans="1:9" ht="68">
-      <c r="A60" s="1" t="s">
-        <v>191</v>
-      </c>
-      <c r="B60" s="1">
-        <v>2017</v>
-      </c>
-      <c r="C60" s="1" t="s">
-        <v>214</v>
-      </c>
-      <c r="D60" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="E60" s="1">
-        <v>9</v>
-      </c>
       <c r="F60" s="1">
-        <v>2</v>
-      </c>
-      <c r="G60" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="I60" s="1" t="s">
-        <v>106</v>
+        <v>3</v>
+      </c>
+      <c r="H60" s="1" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="61" spans="1:9" ht="51">
       <c r="A61" s="1" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B61" s="1">
-        <v>2017</v>
+        <v>2018</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>215</v>
+        <v>65</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>11</v>
+        <v>66</v>
       </c>
       <c r="E61" s="1">
-        <v>60</v>
-      </c>
-      <c r="G61" s="4" t="s">
-        <v>69</v>
+        <v>143</v>
+      </c>
+      <c r="F61" s="1">
+        <v>5</v>
       </c>
       <c r="H61" s="1" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="62" spans="1:9" ht="51">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" ht="68">
       <c r="A62" s="1" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="B62" s="1">
         <v>2017</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="E62" s="1">
-        <v>140</v>
+        <v>9</v>
       </c>
       <c r="F62" s="1">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="G62" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="H62" s="1" t="s">
-        <v>139</v>
+        <v>68</v>
       </c>
       <c r="I62" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="63" spans="1:9" ht="51">
       <c r="A63" s="1" t="s">
-        <v>193</v>
+        <v>163</v>
       </c>
       <c r="B63" s="1">
         <v>2017</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>72</v>
+        <v>11</v>
       </c>
       <c r="E63" s="1">
-        <v>10</v>
+        <v>60</v>
       </c>
       <c r="G63" s="4" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="H63" s="1" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="64" spans="1:9" ht="68">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" ht="51">
       <c r="A64" s="1" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="B64" s="1">
         <v>2017</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>74</v>
+        <v>214</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>36</v>
+        <v>70</v>
       </c>
       <c r="E64" s="1">
-        <v>111</v>
+        <v>140</v>
       </c>
       <c r="F64" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G64" s="4" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="H64" s="1" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="65" spans="1:8" ht="68">
+        <v>137</v>
+      </c>
+      <c r="I64" s="1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8" ht="51">
       <c r="A65" s="1" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="B65" s="1">
         <v>2017</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="E65" s="1">
-        <v>55</v>
+        <v>10</v>
       </c>
       <c r="G65" s="4" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="H65" s="1" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="66" spans="1:8" ht="51">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8" ht="68">
       <c r="A66" s="1" t="s">
-        <v>185</v>
+        <v>192</v>
       </c>
       <c r="B66" s="1">
         <v>2017</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>81</v>
+        <v>36</v>
       </c>
       <c r="E66" s="1">
-        <v>36</v>
+        <v>111</v>
       </c>
       <c r="F66" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G66" s="4" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="H66" s="1" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="67" spans="1:8" ht="51">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8" ht="68">
       <c r="A67" s="1" t="s">
-        <v>165</v>
+        <v>193</v>
       </c>
       <c r="B67" s="1">
         <v>2017</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>84</v>
+        <v>216</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>11</v>
+        <v>78</v>
       </c>
       <c r="E67" s="1">
-        <v>60</v>
-      </c>
-      <c r="F67" s="1">
-        <v>3</v>
+        <v>55</v>
       </c>
       <c r="G67" s="4" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="H67" s="1" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="68" spans="1:8" ht="34">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8" ht="51">
       <c r="A68" s="1" t="s">
-        <v>196</v>
+        <v>183</v>
       </c>
       <c r="B68" s="1">
         <v>2017</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>219</v>
+        <v>80</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="E68" s="1">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="F68" s="1">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="G68" s="4" t="s">
-        <v>88</v>
+        <v>82</v>
+      </c>
+      <c r="H68" s="1" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="69" spans="1:8" ht="51">
       <c r="A69" s="1" t="s">
-        <v>192</v>
+        <v>163</v>
       </c>
       <c r="B69" s="1">
-        <v>2016</v>
+        <v>2017</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>220</v>
+        <v>84</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>61</v>
+        <v>11</v>
       </c>
       <c r="E69" s="1">
-        <v>1</v>
+        <v>60</v>
       </c>
       <c r="F69" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G69" s="4" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="70" spans="1:8" ht="34">
+        <v>85</v>
+      </c>
+      <c r="H69" s="1" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8" ht="51">
       <c r="A70" s="1" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="B70" s="1">
-        <v>2016</v>
+        <v>2017</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>61</v>
+        <v>87</v>
       </c>
       <c r="E70" s="1">
-        <v>1</v>
+        <v>30</v>
       </c>
       <c r="F70" s="1">
         <v>2</v>
       </c>
       <c r="G70" s="4" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="71" spans="1:8" ht="34">
+        <v>88</v>
+      </c>
+      <c r="H70" s="1" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8" ht="51">
       <c r="A71" s="1" t="s">
-        <v>198</v>
+        <v>190</v>
       </c>
       <c r="B71" s="1">
         <v>2016</v>
       </c>
       <c r="C71" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="D71" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="E71" s="1">
+        <v>1</v>
+      </c>
+      <c r="F71" s="1">
+        <v>2</v>
+      </c>
+      <c r="G71" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="H71" s="1" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="72" spans="1:8" ht="51">
+      <c r="A72" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="B72" s="1">
+        <v>2016</v>
+      </c>
+      <c r="C72" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="D72" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="E72" s="1">
+        <v>1</v>
+      </c>
+      <c r="F72" s="1">
+        <v>2</v>
+      </c>
+      <c r="G72" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="H72" s="1" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8" ht="68">
+      <c r="A73" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="B73" s="1">
+        <v>2016</v>
+      </c>
+      <c r="C73" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="D73" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="E73" s="1">
+        <v>37</v>
+      </c>
+      <c r="F73" s="1">
+        <v>6</v>
+      </c>
+      <c r="G73" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="H73" s="1" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8" ht="68">
+      <c r="A74" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="B74" s="1">
+        <v>2015</v>
+      </c>
+      <c r="C74" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="D74" s="1" t="s">
         <v>222</v>
       </c>
-      <c r="D71" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="E71" s="1">
-        <v>37</v>
-      </c>
-      <c r="F71" s="1">
-        <v>6</v>
-      </c>
-      <c r="G71" s="4" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="72" spans="1:8" ht="68">
-      <c r="A72" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="B72" s="1">
-        <v>2015</v>
-      </c>
-      <c r="C72" s="1" t="s">
-        <v>223</v>
-      </c>
-      <c r="D72" s="1" t="s">
-        <v>224</v>
-      </c>
-      <c r="E72" s="1">
+      <c r="E74" s="1">
         <v>115</v>
       </c>
-      <c r="F72" s="1">
+      <c r="F74" s="1">
         <v>5</v>
       </c>
-      <c r="G72" s="4" t="s">
+      <c r="G74" s="4" t="s">
         <v>93</v>
+      </c>
+      <c r="H74" s="1" t="s">
+        <v>349</v>
       </c>
     </row>
   </sheetData>
@@ -3064,6 +3527,283 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3DB5C68-0218-0246-B22C-8D069C454BCB}">
+  <dimension ref="A1:J8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="1" max="1" width="30.1640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="36" style="1" customWidth="1"/>
+    <col min="3" max="3" width="12.1640625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="42.33203125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="13" style="1" customWidth="1"/>
+    <col min="6" max="6" width="11.5" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="10.83203125" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" ht="17">
+      <c r="A1" s="2" t="s">
+        <v>359</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>385</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>386</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>350</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>357</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>351</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="34">
+      <c r="A2" s="1" t="s">
+        <v>360</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>354</v>
+      </c>
+      <c r="C2" s="1">
+        <v>2023</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>353</v>
+      </c>
+      <c r="E2" s="14">
+        <v>45108</v>
+      </c>
+      <c r="F2" s="14">
+        <v>46934</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>355</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>356</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>358</v>
+      </c>
+      <c r="J2" s="13">
+        <v>2329452</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="34">
+      <c r="A3" s="1" t="s">
+        <v>363</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>362</v>
+      </c>
+      <c r="C3" s="1">
+        <v>2023</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>361</v>
+      </c>
+      <c r="E3" s="14">
+        <v>45108</v>
+      </c>
+      <c r="F3" s="14">
+        <v>45657</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>363</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>358</v>
+      </c>
+      <c r="J3" s="13">
+        <v>150000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="51">
+      <c r="A4" s="1" t="s">
+        <v>366</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>365</v>
+      </c>
+      <c r="C4" s="1">
+        <v>2020</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>364</v>
+      </c>
+      <c r="E4" s="14">
+        <v>44075</v>
+      </c>
+      <c r="F4" s="14">
+        <v>45534</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>366</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>367</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>358</v>
+      </c>
+      <c r="J4" s="13">
+        <v>2296000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="85">
+      <c r="A5" s="1" t="s">
+        <v>372</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>369</v>
+      </c>
+      <c r="C5" s="1">
+        <v>2020</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>368</v>
+      </c>
+      <c r="E5" s="14">
+        <v>44013</v>
+      </c>
+      <c r="F5" s="14">
+        <v>45473</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>370</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>371</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>358</v>
+      </c>
+      <c r="J5" s="13">
+        <v>499927</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="68">
+      <c r="A6" s="1" t="s">
+        <v>376</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>374</v>
+      </c>
+      <c r="C6" s="1">
+        <v>2020</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>373</v>
+      </c>
+      <c r="E6" s="14">
+        <v>44075</v>
+      </c>
+      <c r="F6" s="14">
+        <v>45169</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>376</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>375</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>358</v>
+      </c>
+      <c r="J6" s="13">
+        <v>1099997</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="34">
+      <c r="A7" s="1" t="s">
+        <v>381</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>378</v>
+      </c>
+      <c r="C7" s="1">
+        <v>2020</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>377</v>
+      </c>
+      <c r="E7" s="14">
+        <v>43922</v>
+      </c>
+      <c r="F7" s="14">
+        <v>45016</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>355</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>379</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>380</v>
+      </c>
+      <c r="J7" s="13">
+        <v>430000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="34">
+      <c r="A8" s="1" t="s">
+        <v>381</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>383</v>
+      </c>
+      <c r="C8" s="1">
+        <v>2020</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>382</v>
+      </c>
+      <c r="E8" s="14">
+        <v>44013</v>
+      </c>
+      <c r="F8" s="14">
+        <v>44742</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>355</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>384</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>380</v>
+      </c>
+      <c r="J8" s="13">
+        <v>420000</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C08510A-9525-3140-B9DE-25CE081DC0F0}">
   <dimension ref="A1"/>
   <sheetViews>

</xml_diff>

<commit_message>
updated teaching page and cv
</commit_message>
<xml_diff>
--- a/assets/CV/pubs.xlsx
+++ b/assets/CV/pubs.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10714"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tysonbarrett/Dropbox/GitHub/blog_rstats/assets/CV/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0ADE2DBD-3F41-9D40-B641-C2B684AD002F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9341755F-97F3-264C-8839-F4148A036D39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4260" yWindow="740" windowWidth="24540" windowHeight="16520" xr2:uid="{D694CAF4-E52C-7242-8187-CC366AD31369}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="510" uniqueCount="449">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="514" uniqueCount="456">
   <si>
     <t>authors</t>
   </si>
@@ -1386,6 +1386,27 @@
   </si>
   <si>
     <t>Impact of Real-World Implementation of Evidence-Based Insomnia Treatment within a Large Payor-Provider Health System: Initial Provider and Patient-Level Outcomes</t>
+  </si>
+  <si>
+    <t>doi: 10.1093/sleepadvances/zpae054</t>
+  </si>
+  <si>
+    <t>577-588</t>
+  </si>
+  <si>
+    <t>1360-1369</t>
+  </si>
+  <si>
+    <t>4861-4863</t>
+  </si>
+  <si>
+    <t>doi: 10.1245/s10434-024-15417-3</t>
+  </si>
+  <si>
+    <t>doi: 10.1371/journal.pone.0302575</t>
+  </si>
+  <si>
+    <t>e0302575</t>
   </si>
 </sst>
 </file>
@@ -1840,7 +1861,7 @@
   <dimension ref="A1:I87"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="A9" sqref="A9:XFD9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1900,6 +1921,9 @@
         <v>447</v>
       </c>
       <c r="G2" s="1"/>
+      <c r="H2" s="1" t="s">
+        <v>246</v>
+      </c>
     </row>
     <row r="3" spans="1:9" ht="68">
       <c r="A3" s="1" t="s">
@@ -1916,159 +1940,200 @@
       </c>
       <c r="G3" s="1"/>
     </row>
-    <row r="4" spans="1:9" ht="34">
+    <row r="4" spans="1:9" ht="51">
       <c r="A4" s="1" t="s">
-        <v>438</v>
+        <v>424</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>296</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>439</v>
+        <v>423</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>441</v>
+        <v>447</v>
       </c>
       <c r="G4" s="1"/>
+      <c r="H4" s="1" t="s">
+        <v>449</v>
+      </c>
     </row>
     <row r="5" spans="1:9" ht="34">
       <c r="A5" s="1" t="s">
-        <v>424</v>
+        <v>426</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>296</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>423</v>
+        <v>428</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>447</v>
+        <v>427</v>
       </c>
       <c r="G5" s="1"/>
     </row>
-    <row r="6" spans="1:9" ht="34">
+    <row r="6" spans="1:9" ht="68">
       <c r="A6" s="1" t="s">
-        <v>426</v>
+        <v>418</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>296</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>428</v>
+        <v>421</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>427</v>
+        <v>419</v>
       </c>
       <c r="G6" s="1"/>
-    </row>
-    <row r="7" spans="1:9" ht="68">
-      <c r="A7" s="15" t="s">
-        <v>425</v>
+      <c r="H6" s="1" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="51">
+      <c r="A7" s="1" t="s">
+        <v>403</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>296</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>429</v>
+        <v>408</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>143</v>
+        <v>404</v>
       </c>
       <c r="G7" s="1"/>
+      <c r="H7" s="1" t="s">
+        <v>434</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>405</v>
+      </c>
     </row>
     <row r="8" spans="1:9" ht="68">
       <c r="A8" s="1" t="s">
-        <v>418</v>
+        <v>387</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>296</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>421</v>
+        <v>407</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>419</v>
+        <v>388</v>
       </c>
       <c r="G8" s="1"/>
       <c r="H8" s="1" t="s">
-        <v>436</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" ht="51">
-      <c r="A9" s="1" t="s">
-        <v>415</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>296</v>
+        <v>433</v>
+      </c>
+      <c r="I8" s="10"/>
+    </row>
+    <row r="9" spans="1:9" ht="68">
+      <c r="A9" s="15" t="s">
+        <v>425</v>
+      </c>
+      <c r="B9" s="1">
+        <v>2024</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>420</v>
+        <v>429</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="G9" s="1"/>
+        <v>143</v>
+      </c>
+      <c r="E9" s="1">
+        <v>19</v>
+      </c>
+      <c r="F9" s="1">
+        <v>4</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>455</v>
+      </c>
       <c r="H9" s="1" t="s">
-        <v>437</v>
+        <v>454</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="51">
       <c r="A10" s="1" t="s">
-        <v>390</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>296</v>
+        <v>438</v>
+      </c>
+      <c r="B10" s="1">
+        <v>2024</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>409</v>
+        <v>439</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>389</v>
-      </c>
-      <c r="G10" s="1"/>
+        <v>441</v>
+      </c>
+      <c r="E10" s="1">
+        <v>31</v>
+      </c>
+      <c r="F10" s="1">
+        <v>8</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>452</v>
+      </c>
       <c r="H10" s="1" t="s">
-        <v>406</v>
+        <v>453</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="51">
       <c r="A11" s="1" t="s">
-        <v>403</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>296</v>
+        <v>415</v>
+      </c>
+      <c r="B11" s="1">
+        <v>2024</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>408</v>
+        <v>420</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>404</v>
-      </c>
-      <c r="G11" s="1"/>
+        <v>11</v>
+      </c>
+      <c r="E11" s="1">
+        <v>67</v>
+      </c>
+      <c r="F11" s="1">
+        <v>5</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>451</v>
+      </c>
       <c r="H11" s="1" t="s">
-        <v>434</v>
-      </c>
-      <c r="I11" s="1" t="s">
-        <v>405</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" ht="68">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="51">
       <c r="A12" s="1" t="s">
-        <v>387</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>296</v>
+        <v>390</v>
+      </c>
+      <c r="B12" s="1">
+        <v>2024</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>407</v>
+        <v>409</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>388</v>
-      </c>
-      <c r="G12" s="1"/>
+        <v>389</v>
+      </c>
+      <c r="E12" s="1">
+        <v>131</v>
+      </c>
+      <c r="F12" s="1">
+        <v>5</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>450</v>
+      </c>
       <c r="H12" s="1" t="s">
-        <v>433</v>
-      </c>
-      <c r="I12" s="10"/>
+        <v>406</v>
+      </c>
     </row>
     <row r="13" spans="1:9" ht="51">
       <c r="A13" s="1" t="s">

</xml_diff>

<commit_message>
updated cv and pydata
</commit_message>
<xml_diff>
--- a/assets/CV/pubs.xlsx
+++ b/assets/CV/pubs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11013"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11207"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tysonbarrett/Dropbox/GitHub/blog_rstats/assets/CV/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96140D0C-C5F2-894C-B7E2-97509AFC806D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94AB394A-B8E0-A842-95F7-D3E6A715F705}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2240" yWindow="740" windowWidth="24540" windowHeight="16520" activeTab="1" xr2:uid="{D694CAF4-E52C-7242-8187-CC366AD31369}"/>
+    <workbookView xWindow="2240" yWindow="740" windowWidth="24540" windowHeight="16520" xr2:uid="{D694CAF4-E52C-7242-8187-CC366AD31369}"/>
   </bookViews>
   <sheets>
     <sheet name="Journals" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="535" uniqueCount="471">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="537" uniqueCount="476">
   <si>
     <t>authors</t>
   </si>
@@ -1452,6 +1452,21 @@
   </si>
   <si>
     <t>R01DC020930</t>
+  </si>
+  <si>
+    <t>41-47</t>
+  </si>
+  <si>
+    <t>doi: 10.1016/j.jad.2024.09.056</t>
+  </si>
+  <si>
+    <t>zpae053</t>
+  </si>
+  <si>
+    <t>doi: 10.1093/sleepadvances/zpae053</t>
+  </si>
+  <si>
+    <t>doi: 10.1037/sah0000543</t>
   </si>
 </sst>
 </file>
@@ -1916,8 +1931,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38BAB23D-B27F-A34D-A522-4C115B575C05}">
   <dimension ref="A1:I91"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1981,33 +1996,30 @@
         <v>465</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="68">
+    <row r="3" spans="1:9" ht="34">
       <c r="A3" s="1" t="s">
-        <v>424</v>
+        <v>461</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>296</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>457</v>
+        <v>462</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>447</v>
+        <v>145</v>
       </c>
       <c r="G3" s="1"/>
-      <c r="H3" s="1" t="s">
-        <v>246</v>
-      </c>
     </row>
     <row r="4" spans="1:9" ht="34">
       <c r="A4" s="1" t="s">
-        <v>461</v>
+        <v>455</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>296</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>462</v>
+        <v>456</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>145</v>
@@ -2016,48 +2028,70 @@
     </row>
     <row r="5" spans="1:9" ht="68">
       <c r="A5" s="1" t="s">
-        <v>459</v>
+        <v>442</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>296</v>
       </c>
       <c r="C5" s="1" t="s">
+        <v>440</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>435</v>
+      </c>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1" t="s">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="68">
+      <c r="A6" s="1" t="s">
+        <v>459</v>
+      </c>
+      <c r="B6" s="1">
+        <v>2025</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>460</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="D6" s="1" t="s">
         <v>458</v>
       </c>
-      <c r="G5" s="1"/>
-    </row>
-    <row r="6" spans="1:9" ht="34">
-      <c r="A6" s="1" t="s">
-        <v>455</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>296</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>456</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="G6" s="1"/>
+      <c r="E6" s="1">
+        <v>368</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>471</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>472</v>
+      </c>
     </row>
     <row r="7" spans="1:9" ht="68">
       <c r="A7" s="1" t="s">
-        <v>442</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>296</v>
+        <v>424</v>
+      </c>
+      <c r="B7" s="1">
+        <v>2024</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>440</v>
+        <v>457</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>435</v>
-      </c>
-      <c r="G7" s="1"/>
+        <v>447</v>
+      </c>
+      <c r="E7" s="1">
+        <v>5</v>
+      </c>
+      <c r="F7" s="1">
+        <v>1</v>
+      </c>
+      <c r="G7" s="17" t="s">
+        <v>473</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>474</v>
+      </c>
     </row>
     <row r="8" spans="1:9" ht="51">
       <c r="A8" s="1" t="s">
@@ -2071,6 +2105,12 @@
       </c>
       <c r="D8" s="1" t="s">
         <v>447</v>
+      </c>
+      <c r="E8" s="1">
+        <v>5</v>
+      </c>
+      <c r="F8" s="1">
+        <v>1</v>
       </c>
       <c r="G8" s="17" t="s">
         <v>467</v>
@@ -4225,7 +4265,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3DB5C68-0218-0246-B22C-8D069C454BCB}">
   <dimension ref="A1:J10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>

</xml_diff>